<commit_message>
#8867 - update test, toFixed not the same as round
</commit_message>
<xml_diff>
--- a/db/test_data/im_data_test.xlsx
+++ b/db/test_data/im_data_test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwestphal\Projects\doc\internet_monitor\db\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Projects\doc\internet_monitor\db\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="0" windowWidth="27540" windowHeight="14310"/>
+    <workbookView xWindow="2190" yWindow="0" windowWidth="27540" windowHeight="14310"/>
   </bookViews>
   <sheets>
     <sheet name="im_data_test" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">im_data_test!$A$1:$L$23</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -181,6 +181,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -660,7 +663,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -985,8 +988,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1004,7 @@
     <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1038,7 +1041,7 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1076,7 +1079,7 @@
       <c r="K2">
         <v>30.8539009094</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1152,7 +1155,7 @@
       <c r="K4">
         <v>3.41114943653143E-3</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1190,7 +1193,7 @@
       <c r="K5">
         <v>8802.5113333333302</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1228,7 +1231,7 @@
       <c r="K6">
         <v>94.272199999999998</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1415,7 +1418,7 @@
       <c r="K11">
         <v>21</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1453,7 +1456,7 @@
       <c r="K12">
         <v>48.37482</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1529,7 +1532,7 @@
       <c r="K14">
         <v>3.6604822758688599E-3</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1605,7 +1608,7 @@
       <c r="K16">
         <v>36.518400270000001</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1827,7 +1830,7 @@
       <c r="K22">
         <v>77.863</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="1">
         <v>5.7706080589623401</v>
       </c>
     </row>
@@ -1865,7 +1868,7 @@
       <c r="K23">
         <v>65.477346786400005</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1876,7 +1879,7 @@
       <c r="E24" t="s">
         <v>16</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="1">
         <f>AVERAGE(L11*I11 + IF(I11 &lt; 0, 1, 0),L12*I12 + IF(I12 &lt; 0, 1, 0))</f>
         <v>0.25</v>
       </c>
@@ -1888,7 +1891,7 @@
       <c r="E25" t="s">
         <v>20</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="1">
         <f>AVERAGE(L14*I14+IF(I14&lt;0,1,0))</f>
         <v>1</v>
       </c>
@@ -1900,7 +1903,7 @@
       <c r="E26" t="s">
         <v>25</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="1">
         <f>AVERAGE(L15*I15 + IF(I15 &lt; 0, 1, 0))</f>
         <v>-4.5459079847434203E-16</v>
       </c>
@@ -1912,7 +1915,7 @@
       <c r="E27" t="s">
         <v>29</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="1">
         <f>AVERAGE(L16*I16 + IF(I16 &lt; 0, 1, 0))</f>
         <v>0</v>
       </c>
@@ -1924,7 +1927,7 @@
       <c r="E28" t="s">
         <v>50</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="1">
         <f>AVERAGE(L24:L27)*10</f>
         <v>3.1249999999999991</v>
       </c>
@@ -1936,7 +1939,7 @@
       <c r="E29" t="s">
         <v>16</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="1">
         <f>AVERAGE(L2*I2+IF(I2&lt;0,1,0))</f>
         <v>1</v>
       </c>
@@ -1948,7 +1951,7 @@
       <c r="E30" t="s">
         <v>20</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="1">
         <f>AVERAGE(L3*I3+IF(I3&lt;0,1,0))</f>
         <v>1</v>
       </c>
@@ -1960,7 +1963,7 @@
       <c r="E31" t="s">
         <v>25</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="1">
         <f>AVERAGE(L3*I3 + IF(I3 &lt; 0, 1, 0))</f>
         <v>1</v>
       </c>
@@ -1972,7 +1975,7 @@
       <c r="E32" t="s">
         <v>29</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="1">
         <f>AVERAGE(L4*I4 + IF(I4 &lt; 0, 1, 0))</f>
         <v>0</v>
       </c>
@@ -1984,7 +1987,7 @@
       <c r="E33" t="s">
         <v>50</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="1">
         <f>AVERAGE(L29:L32)*10</f>
         <v>7.5</v>
       </c>
@@ -1998,5 +2001,6 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>